<commit_message>
adding duplicate email verification testcase
</commit_message>
<xml_diff>
--- a/PHPTravelTests/Data/Data.xlsx
+++ b/PHPTravelTests/Data/Data.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationPageTests" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>FirstName</t>
   </si>
@@ -49,12 +49,15 @@
   </si>
   <si>
     <t>hamada</t>
+  </si>
+  <si>
+    <t>add_TwoUsers_With_Same_Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -384,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -392,7 +395,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
@@ -437,11 +440,32 @@
         <v>123456</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>123456</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>